<commit_message>
Fin de première phase sql
</commit_message>
<xml_diff>
--- a/database/merise/src/exercice6_inventory_of_works_of_art/doc/data_dictionary.xlsx
+++ b/database/merise/src/exercice6_inventory_of_works_of_art/doc/data_dictionary.xlsx
@@ -5,19 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fturl\Documents\GitHub\FTurleque\abc_2105-perso\base_de_donnee\merise\exercice6_Inventory_of_works_of_art\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fturl\Documents\GitHub\FTurleque\abc_2105-perso\database\merise\src\exercice6_inventory_of_works_of_art\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{728BCC8B-1388-467E-BF9C-E1CF6D7507BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28189751-5FA9-457B-9D4E-A62422EF20F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="inventory_of_works" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_Hlk80949070" localSheetId="0">Feuil1!$A$9</definedName>
-    <definedName name="_Hlk80949108" localSheetId="0">Feuil1!$A$11</definedName>
+    <definedName name="_Hlk80949070" localSheetId="0">inventory_of_works!$A$10</definedName>
+    <definedName name="_Hlk80949108" localSheetId="0">inventory_of_works!$A$12</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="60">
   <si>
     <t>Mnémonique</t>
   </si>
@@ -203,6 +203,12 @@
   </si>
   <si>
     <t>AN</t>
+  </si>
+  <si>
+    <t>work_material</t>
+  </si>
+  <si>
+    <t>Matière qui compose l'œuvre.</t>
   </si>
 </sst>
 </file>
@@ -248,15 +254,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -271,13 +275,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD2D2D2"/>
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE8E8E8"/>
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -346,7 +362,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -354,7 +370,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -366,7 +382,13 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -375,13 +397,46 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -664,15 +719,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
@@ -717,16 +772,16 @@
       <c r="A3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="9">
+      <c r="C3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="5">
         <v>24</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="5" t="s">
         <v>12</v>
       </c>
     </row>
@@ -751,14 +806,14 @@
       <c r="A5" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="9" t="s">
+      <c r="D5" s="8"/>
+      <c r="E5" s="5" t="s">
         <v>18</v>
       </c>
     </row>
@@ -766,16 +821,16 @@
       <c r="A6" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="9">
-        <v>11</v>
-      </c>
-      <c r="E6" s="9" t="s">
+      <c r="D6" s="5">
+        <v>11</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>12</v>
       </c>
     </row>
@@ -783,16 +838,16 @@
       <c r="A7" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="9">
-        <v>11</v>
-      </c>
-      <c r="E7" s="9" t="s">
+      <c r="D7" s="5">
+        <v>11</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>12</v>
       </c>
     </row>
@@ -800,246 +855,263 @@
       <c r="A8" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="9">
-        <v>11</v>
-      </c>
-      <c r="E8" s="9" t="s">
+      <c r="D8" s="5">
+        <v>11</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="5">
+        <v>32</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B10" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="9">
-        <v>11</v>
-      </c>
-      <c r="E9" s="9" t="s">
+      <c r="D10" s="5">
+        <v>11</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
+    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B11" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C11" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="9">
-        <v>11</v>
-      </c>
-      <c r="E10" s="11" t="s">
+      <c r="D11" s="11">
+        <v>11</v>
+      </c>
+      <c r="E11" s="12" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
+    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B12" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="9">
+      <c r="C12" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="11">
         <v>48</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E12" s="11" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
+    <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B13" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="9">
+      <c r="C13" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="11">
         <v>48</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="E13" s="11" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
+    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B14" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C14" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="9">
-        <v>11</v>
-      </c>
-      <c r="E13" s="11" t="s">
+      <c r="D14" s="16">
+        <v>11</v>
+      </c>
+      <c r="E14" s="17" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="7" t="s">
+    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B15" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" s="5">
+      <c r="C15" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="16">
         <v>48</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E15" s="16" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
+    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B16" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" s="9">
+      <c r="C16" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="16">
         <v>48</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="E16" s="16" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="7" t="s">
+    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B17" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16" s="9">
+      <c r="C17" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="16">
         <v>48</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="E17" s="16" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="7" t="s">
+    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B18" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C18" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="10"/>
-      <c r="E17" s="9" t="s">
+      <c r="D18" s="19"/>
+      <c r="E18" s="16" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="7" t="s">
+    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B19" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C19" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="10"/>
-      <c r="E18" s="9" t="s">
+      <c r="D19" s="19"/>
+      <c r="E19" s="16" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
+    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B20" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="C19" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" s="9">
+      <c r="C20" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="22">
         <v>24</v>
       </c>
-      <c r="E19" s="11" t="s">
+      <c r="E20" s="23" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="7" t="s">
+    <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B21" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C21" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="D20" s="12"/>
-      <c r="E20" s="5" t="s">
+      <c r="D21" s="25"/>
+      <c r="E21" s="22" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="7" t="s">
+    <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B22" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C22" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="D21" s="10"/>
-      <c r="E21" s="9" t="s">
+      <c r="D22" s="25"/>
+      <c r="E22" s="22" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="7" t="s">
+    <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B23" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C23" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="D22" s="5">
+      <c r="D23" s="22">
         <v>255</v>
       </c>
-      <c r="E22" s="5" t="s">
+      <c r="E23" s="22" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>